<commit_message>
put DFs in dict, navigated possible feature columns
</commit_message>
<xml_diff>
--- a/BalanceSheet/AAPL_bal.xlsx
+++ b/BalanceSheet/AAPL_bal.xlsx
@@ -265,7 +265,7 @@
         <v>95128000000.0</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>107230000000.0</v>
+        <v>107162000000.0</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>100557000000.0</v>
@@ -504,7 +504,7 @@
         </is>
       </c>
       <c r="B4" s="0" t="n">
-        <v>5219000000.0</v>
+        <v>4943000000.0</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>4023000000.0</v>
@@ -519,7 +519,7 @@
         <v>4061000000.0</v>
       </c>
       <c r="G4" s="0" t="n">
-        <v>4069000000.0</v>
+        <v>4097000000.0</v>
       </c>
       <c r="H4" s="0" t="n">
         <v>4106000000.0</v>
@@ -646,7 +646,7 @@
         <v>14614000000.0</v>
       </c>
       <c r="G5" s="0" t="n">
-        <v>11958000000.0</v>
+        <v>12026000000.0</v>
       </c>
       <c r="H5" s="0" t="n">
         <v>12352000000.0</v>
@@ -900,7 +900,7 @@
         <v>43986000000.0</v>
       </c>
       <c r="G7" s="0" t="n">
-        <v>44293000000.0</v>
+        <v>37031000000.0</v>
       </c>
       <c r="H7" s="0" t="n">
         <v>37378000000.0</v>
@@ -1027,7 +1027,7 @@
         <v>100591000000.0</v>
       </c>
       <c r="G8" s="0" t="n">
-        <v>101725000000.0</v>
+        <v>99899000000.0</v>
       </c>
       <c r="H8" s="0" t="n">
         <v>105341000000.0</v>
@@ -1309,7 +1309,7 @@
         <v>32070000000.0</v>
       </c>
       <c r="G10" s="0" t="n">
-        <v>31369000000.0</v>
+        <v>40457000000.0</v>
       </c>
       <c r="H10" s="0" t="n">
         <v>32978000000.0</v>
@@ -1675,7 +1675,7 @@
         </is>
       </c>
       <c r="B13" s="0" t="n">
-        <v>40127000000.0</v>
+        <v>16460000000.0</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>85516000000.0</v>
@@ -1690,7 +1690,7 @@
         <v>19990000000.0</v>
       </c>
       <c r="G13" s="0" t="n">
-        <v>44022000000.0</v>
+        <v>45111000000.0</v>
       </c>
       <c r="H13" s="0" t="n">
         <v>46236000000.0</v>
@@ -1968,7 +1968,7 @@
         <v>21625000000.0</v>
       </c>
       <c r="G15" s="0" t="n">
-        <v>16473000000.0</v>
+        <v>15214000000.0</v>
       </c>
       <c r="H15" s="0" t="n">
         <v>16240000000.0</v>
@@ -2231,7 +2231,7 @@
         </is>
       </c>
       <c r="B17" s="0" t="n">
-        <v>45660000000.0</v>
+        <v>53255000000.0</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>55899000000.0</v>
@@ -2246,7 +2246,7 @@
         <v>42048000000.0</v>
       </c>
       <c r="G17" s="0" t="n">
-        <v>40577000000.0</v>
+        <v>36263000000.0</v>
       </c>
       <c r="H17" s="0" t="n">
         <v>37720000000.0</v>
@@ -2556,7 +2556,7 @@
         <v>97136000000.0</v>
       </c>
       <c r="G19" s="0" t="n">
-        <v>100278000000.0</v>
+        <v>93078000000.0</v>
       </c>
       <c r="H19" s="0" t="n">
         <v>91807000000.0</v>
@@ -2832,10 +2832,8 @@
           <t>Long Term Tax Liability (Deferred)</t>
         </is>
       </c>
-      <c r="B21" s="0" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+      <c r="B21" s="0" t="n">
+        <v>-149000000.0</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>-58000000.0</v>
@@ -3045,7 +3043,7 @@
         <v>48745000000.0</v>
       </c>
       <c r="G22" s="0" t="n">
-        <v>48648000000.0</v>
+        <v>55848000000.0</v>
       </c>
       <c r="H22" s="0" t="n">
         <v>50503000000.0</v>
@@ -4046,7 +4044,7 @@
         </is>
       </c>
       <c r="B30" s="0" t="n">
-        <v>16686310000.0</v>
+        <v>16686300000.0</v>
       </c>
       <c r="C30" s="0" t="n">
         <v>16823260000.0</v>

</xml_diff>

<commit_message>
adding lots of .xlsx files and updating main working notebooks
</commit_message>
<xml_diff>
--- a/BalanceSheet/AAPL_bal.xlsx
+++ b/BalanceSheet/AAPL_bal.xlsx
@@ -4313,7 +4313,7 @@
         <v>23633000000.0</v>
       </c>
       <c r="G32" s="0" t="n">
-        <v>9521000000.0</v>
+        <v>1130000000.0</v>
       </c>
       <c r="H32" s="0" t="n">
         <v>7490000000.0</v>
@@ -4440,7 +4440,7 @@
         <v>118761000000.0</v>
       </c>
       <c r="G33" s="0" t="n">
-        <v>116751000000.0</v>
+        <v>108292000000.0</v>
       </c>
       <c r="H33" s="0" t="n">
         <v>108047000000.0</v>

</xml_diff>